<commit_message>
Add requirements file and update geojson properties for submarine cable data
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,15 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgpeytrignet/Library/CloudStorage/GoogleDrive-peytrignet.sebastien@gmail.com/My Drive/WATRA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgpeytrignet/Library/CloudStorage/GoogleDrive-peytrignet.sebastien@gmail.com/My Drive/WATRA-fiber-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2955AAF-018A-3146-A37B-B7FAAF8699DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC2E25D-766F-8F4E-BB8E-42A3F1894143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{A9F62FD1-5AF6-8B43-9DB1-9C6C60EEBB07}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="5" xr2:uid="{A9F62FD1-5AF6-8B43-9DB1-9C6C60EEBB07}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Nodes and Links - Sources" sheetId="1" r:id="rId1"/>
+    <sheet name="Nodes - Data Schema" sheetId="6" r:id="rId2"/>
+    <sheet name="Links - Data Schema" sheetId="5" r:id="rId3"/>
+    <sheet name="Submarine Cables - Sources" sheetId="2" r:id="rId4"/>
+    <sheet name="Submarine Cables - Schema" sheetId="7" r:id="rId5"/>
+    <sheet name="IXP - Sources" sheetId="3" r:id="rId6"/>
+    <sheet name="IXP - Schema" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="229">
   <si>
     <t>country</t>
   </si>
@@ -338,9 +344,6 @@
     <t>Government - FDSUT (USF)</t>
   </si>
   <si>
-    <t>https://sigtel.ecowas.int/wp-content/uploads/2024/03/Togo_map.png</t>
-  </si>
-  <si>
     <t>Government - Ministre de L'Economie Numérique et de la Transformation Digitale</t>
   </si>
   <si>
@@ -363,13 +366,376 @@
   </si>
   <si>
     <t>lines/BEN_lines.geojson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sigtel.ecowas.int/wp-content/uploads/2024/03/Togo_map.png </t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Cabo Verde Telecom Domestic Submarine Cable Phase 2</t>
+  </si>
+  <si>
+    <t>Cabo Verde Telecom Domestic Submarine Cable Phase 3</t>
+  </si>
+  <si>
+    <t>Cabo Verde Telecom Domestic Submarine Cable Phase 1</t>
+  </si>
+  <si>
+    <t>Senegal Horn of Africa Regional Express (SHARE) Cable</t>
+  </si>
+  <si>
+    <t>Nigeria Cameroon Submarine Cable System (NCSCS)</t>
+  </si>
+  <si>
+    <t>EllaLink</t>
+  </si>
+  <si>
+    <t>ATLANTIS-2</t>
+  </si>
+  <si>
+    <t>Maroc Telecom West Africa</t>
+  </si>
+  <si>
+    <t>Glo-1</t>
+  </si>
+  <si>
+    <t>SAT-3/WASC</t>
+  </si>
+  <si>
+    <t>MainOne</t>
+  </si>
+  <si>
+    <t>West Africa Cable System (WACS)</t>
+  </si>
+  <si>
+    <t>Equiano</t>
+  </si>
+  <si>
+    <t>Africa Coast to Europe (ACE)</t>
+  </si>
+  <si>
+    <t>2Africa</t>
+  </si>
+  <si>
+    <t>cable_name</t>
+  </si>
+  <si>
+    <t>source_1</t>
+  </si>
+  <si>
+    <t>source_2</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/2Africa</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Africa_Coast_to_Europe_(cable_system)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/EllaLink</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Equiano_(submarine_communications_cable)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Main_One</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/SAT-3/WASC_(cable_system)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/West_Africa_Cable_System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.submarinecablemap.com/ </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Atlantis-2</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/GLO-1</t>
+  </si>
+  <si>
+    <t>BENINIX</t>
+  </si>
+  <si>
+    <t>BFIX</t>
+  </si>
+  <si>
+    <t>CIVIX</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>SIXP</t>
+  </si>
+  <si>
+    <t>Accra-IX</t>
+  </si>
+  <si>
+    <t>GIX</t>
+  </si>
+  <si>
+    <t>Guinee</t>
+  </si>
+  <si>
+    <t>IXP-GUINEE</t>
+  </si>
+  <si>
+    <t>LIXP</t>
+  </si>
+  <si>
+    <t>MLIX</t>
+  </si>
+  <si>
+    <t>IXPN-Abuja</t>
+  </si>
+  <si>
+    <t>AMS-IX Lagos</t>
+  </si>
+  <si>
+    <t>IXPN-Lagos</t>
+  </si>
+  <si>
+    <t>IXPN-Port Harcourt</t>
+  </si>
+  <si>
+    <t>SENIX</t>
+  </si>
+  <si>
+    <t>TGIX</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>https://af-ix.org/</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Mandatory/Optional</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Node identificator</t>
+  </si>
+  <si>
+    <t>FN12345</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Geographical latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>Geographical longitude</t>
+  </si>
+  <si>
+    <t>operator_name</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Name of the mobile operator</t>
+  </si>
+  <si>
+    <t>TelOperator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure_type </t>
+  </si>
+  <si>
+    <t>Type of Infrastructure: fiber, microwave, other (specify)</t>
+  </si>
+  <si>
+    <t>Fiber</t>
+  </si>
+  <si>
+    <t>node_status</t>
+  </si>
+  <si>
+    <t>Operational</t>
+  </si>
+  <si>
+    <t>equipped_capacity_mbps</t>
+  </si>
+  <si>
+    <t>potential_capacity_mbps</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>data_source_year</t>
+  </si>
+  <si>
+    <t>Source of original data</t>
+  </si>
+  <si>
+    <t>Year data was published</t>
+  </si>
+  <si>
+    <t>NCC</t>
+  </si>
+  <si>
+    <t>Equipped capacity here refers to the bandwidth in telecommunication network where it has been turned on and is ready for use to connect subscribers to the node. Excluding bachhaul equipped capacity.</t>
+  </si>
+  <si>
+    <t>Potential capacity here refers to the total theoretical bandwidth that is available for use to connect subscribers to the node. Excluding bachhaul potential capacity.</t>
+  </si>
+  <si>
+    <t>Operational, Planned, Under Construction</t>
+  </si>
+  <si>
+    <t>Country where the link is located</t>
+  </si>
+  <si>
+    <t>Country where the node is located</t>
+  </si>
+  <si>
+    <t>Regional classification</t>
+  </si>
+  <si>
+    <t>line_id</t>
+  </si>
+  <si>
+    <t>Line/link identificator</t>
+  </si>
+  <si>
+    <t>FL12345</t>
+  </si>
+  <si>
+    <t>Name of the telecommunications operator or infrastructure provider</t>
+  </si>
+  <si>
+    <t>MTN, Orange, Airtel</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>Starting node identifier or location name</t>
+  </si>
+  <si>
+    <t>Ending node identifier or location name</t>
+  </si>
+  <si>
+    <t>Lagos</t>
+  </si>
+  <si>
+    <t>Abuja</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>Physical distance of the link in meters</t>
+  </si>
+  <si>
+    <t>Source organization or entity that published the original data</t>
+  </si>
+  <si>
+    <t>NCC, World Bank, ECOWAS</t>
+  </si>
+  <si>
+    <t>Year the data was published or collected</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Name of the submarine cable system</t>
+  </si>
+  <si>
+    <t>ACE (Africa Coast to Europe), MainOne, SAT-3/WASC</t>
+  </si>
+  <si>
+    <t>capacity_Tbps</t>
+  </si>
+  <si>
+    <t>Total design capacity of the submarine cable system in Terabits per second</t>
+  </si>
+  <si>
+    <t>year_service</t>
+  </si>
+  <si>
+    <t>Year the submarine cable entered commercial service</t>
+  </si>
+  <si>
+    <t>length_km</t>
+  </si>
+  <si>
+    <t>Total length of the submarine cable system in kilometers</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Cables</t>
+  </si>
+  <si>
+    <t>Landing Station</t>
+  </si>
+  <si>
+    <t>cables_count</t>
+  </si>
+  <si>
+    <t>first_cable_name</t>
+  </si>
+  <si>
+    <t>Name of the landing station</t>
+  </si>
+  <si>
+    <t>Accra, Ghana</t>
+  </si>
+  <si>
+    <t>Number of cables that use the landing station</t>
+  </si>
+  <si>
+    <t>Name of the first cable</t>
+  </si>
+  <si>
+    <t>Africa1</t>
+  </si>
+  <si>
+    <t>Name of the Internet Exchange Point</t>
+  </si>
+  <si>
+    <t>Country where the IXP is located</t>
+  </si>
+  <si>
+    <t>BENIN-IX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -389,6 +755,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,11 +788,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -737,13 +1124,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670B1EDA-0E58-C54A-8B7B-3A324331E1D9}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="20.83203125" customWidth="1"/>
+    <col min="1" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -902,7 +1289,7 @@
         <v>39</v>
       </c>
       <c r="D6">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="E6" t="s">
         <v>35</v>
@@ -1156,11 +1543,11 @@
       <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
         <v>100</v>
-      </c>
-      <c r="C15" t="s">
-        <v>101</v>
       </c>
       <c r="D15" t="s">
         <v>87</v>
@@ -1169,13 +1556,13 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" t="s">
         <v>102</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>103</v>
-      </c>
-      <c r="H15" t="s">
-        <v>104</v>
       </c>
       <c r="I15" s="2">
         <v>45839</v>
@@ -1186,7 +1573,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1198,13 +1585,13 @@
         <v>35</v>
       </c>
       <c r="F16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" t="s">
         <v>106</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>107</v>
-      </c>
-      <c r="H16" t="s">
-        <v>108</v>
       </c>
       <c r="I16" s="2">
         <v>45839</v>
@@ -1256,7 +1643,977 @@
     <hyperlink ref="B14" r:id="rId13" xr:uid="{972B4158-B5DE-D14A-B085-97FBCFCDB0EC}"/>
     <hyperlink ref="B5" r:id="rId14" xr:uid="{47493A6C-5FC2-4A47-B405-A47750642764}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{B472A8AA-CE5C-784A-9B82-DEB64187F48A}"/>
+    <hyperlink ref="B15" r:id="rId16" xr:uid="{E87A0F72-4ABC-EB4B-A84E-9DBA4D95AEDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485ADD58-4996-1B48-9971-8CE90CEE2909}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="6">
+        <v>38.988754999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.4019379999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F29216-7309-DD43-8DFB-DECD3E4C0AEC}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6">
+        <v>5230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128E263C-3BB6-C149-A08A-996273D43A8A}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CB9E5CC3-6F90-484E-B6F4-DB261E5D28C5}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{32955101-50F1-8E42-8067-3CE96F7BE223}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{AC371DFD-B6AE-4C4B-89EC-2535F3485797}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{A5DF4D22-F796-3D42-AB26-38E4F845EB57}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{0A3EBA03-CF32-E048-8EFE-D474C1C18F82}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{FE29D1A1-2AC6-994E-A98B-3A056174478C}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{0955D55A-78A4-E545-8039-F4844DEDD11A}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{5ADD6690-5BB4-E348-931E-F01EC187E23C}"/>
+    <hyperlink ref="C3:C16" r:id="rId9" display="https://www.submarinecablemap.com/ " xr:uid="{B86D88D4-99F4-F64E-A41B-FE8FF0613EBC}"/>
+    <hyperlink ref="B4" r:id="rId10" xr:uid="{7F5A7C53-4E50-9245-A18E-47472CA611D5}"/>
+    <hyperlink ref="B10" r:id="rId11" xr:uid="{ED7B586D-FDBC-F141-8676-848E6FA8AA74}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E307F2-751A-8145-9AC7-69157B6ED69F}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4">
+        <v>2020</v>
+      </c>
+      <c r="E4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A19FBA-D762-F041-A02A-E6AD72D8718F}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{657F7916-9654-9147-9B3F-863DA794C931}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494B8C61-10DB-B74D-8F25-E0C69F49F85E}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>